<commit_message>
we get better results using gradient descent for logreg than adadelta; report losses
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>method</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>neural net</t>
+  </si>
+  <si>
+    <t>start lr</t>
+  </si>
+  <si>
+    <t>end lr</t>
   </si>
 </sst>
 </file>
@@ -917,7 +923,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,7 +1237,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -1242,9 +1248,11 @@
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1255,10 +1263,16 @@
         <v>21</v>
       </c>
       <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1266,10 +1280,16 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <v>0.19872000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>0.1</v>
+      </c>
+      <c r="F2">
+        <v>0.19988</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1277,10 +1297,16 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <v>0.13252</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+      <c r="F3">
+        <v>0.13303999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1288,10 +1314,16 @@
         <v>22</v>
       </c>
       <c r="D4">
-        <v>0.13216</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>0.1</v>
+      </c>
+      <c r="F4">
+        <v>0.13156000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1302,10 +1334,16 @@
         <v>22</v>
       </c>
       <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>0.13496</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1316,10 +1354,16 @@
         <v>22</v>
       </c>
       <c r="D6">
-        <v>0.13496</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0.13456000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1330,7 +1374,13 @@
         <v>22</v>
       </c>
       <c r="D7">
-        <v>0.13539999999999999</v>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0.13447999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
predicting the end word gives better results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="doc vecs" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>method</t>
   </si>
@@ -79,12 +79,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>batch sampling</t>
-  </si>
-  <si>
-    <t>docs, unique docs per batch</t>
-  </si>
-  <si>
     <t>logreg</t>
   </si>
   <si>
@@ -94,19 +88,28 @@
     <t>dbow + pvdm</t>
   </si>
   <si>
-    <t>all</t>
-  </si>
-  <si>
     <t>layer sizes</t>
   </si>
   <si>
     <t>neural net</t>
   </si>
   <si>
-    <t>start lr</t>
-  </si>
-  <si>
-    <t>end lr</t>
+    <t>lr</t>
+  </si>
+  <si>
+    <t>epoch size</t>
+  </si>
+  <si>
+    <t>train lr</t>
+  </si>
+  <si>
+    <t>val lr</t>
+  </si>
+  <si>
+    <t>window size</t>
+  </si>
+  <si>
+    <t>end</t>
   </si>
 </sst>
 </file>
@@ -590,15 +593,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -920,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,14 +931,16 @@
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -951,26 +953,32 @@
       <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>18</v>
+      <c r="E1" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -983,26 +991,32 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>19</v>
+      <c r="E2">
+        <v>10</v>
       </c>
       <c r="F2">
+        <v>1E-3</v>
+      </c>
+      <c r="G2">
+        <v>1E-3</v>
+      </c>
+      <c r="H2">
         <v>20</v>
       </c>
-      <c r="G2" s="2">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0.14097222222222222</v>
-      </c>
-      <c r="I2" s="1">
-        <v>3.2638888888888891E-2</v>
-      </c>
-      <c r="J2">
-        <v>0.27279999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I2" s="2">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.10208333333333335</v>
+      </c>
+      <c r="K2" s="1">
+        <v>2.013888888888889E-2</v>
+      </c>
+      <c r="L2">
+        <v>0.24923999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1015,26 +1029,32 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
-        <v>19</v>
+      <c r="E3">
+        <v>10</v>
       </c>
       <c r="F3">
+        <v>1E-3</v>
+      </c>
+      <c r="G3">
+        <v>1E-3</v>
+      </c>
+      <c r="H3">
         <v>20</v>
       </c>
-      <c r="G3" s="2">
-        <v>5</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.11041666666666666</v>
-      </c>
-      <c r="I3" s="1">
-        <v>3.0555555555555555E-2</v>
-      </c>
-      <c r="J3">
-        <v>0.2014</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="2">
+        <v>10</v>
+      </c>
+      <c r="J3" s="1">
+        <v>8.0555555555555561E-2</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="L3">
+        <v>0.20671999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1047,26 +1067,32 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
-        <v>19</v>
+      <c r="E4">
+        <v>10</v>
       </c>
       <c r="F4">
+        <v>1E-3</v>
+      </c>
+      <c r="G4">
+        <v>1E-3</v>
+      </c>
+      <c r="H4">
         <v>20</v>
       </c>
-      <c r="G4" s="2">
-        <v>5</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0.11458333333333333</v>
-      </c>
-      <c r="I4" s="1">
-        <v>2.9166666666666664E-2</v>
-      </c>
-      <c r="J4">
-        <v>0.19284000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="2">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1.5972222222222224E-2</v>
+      </c>
+      <c r="L4">
+        <v>0.19819999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1079,26 +1105,32 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
+      <c r="E5">
+        <v>10</v>
       </c>
       <c r="F5">
+        <v>1E-3</v>
+      </c>
+      <c r="G5">
+        <v>1E-3</v>
+      </c>
+      <c r="H5">
         <v>20</v>
       </c>
-      <c r="G5" s="2">
-        <v>5</v>
-      </c>
-      <c r="H5" s="1">
-        <v>7.8472222222222221E-2</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1.9444444444444445E-2</v>
-      </c>
-      <c r="J5">
-        <v>0.19375999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="2">
+        <v>10</v>
+      </c>
+      <c r="J5" s="1">
+        <v>5.6944444444444443E-2</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="L5">
+        <v>0.20535999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1111,26 +1143,32 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
-        <v>19</v>
+      <c r="E6">
+        <v>10</v>
       </c>
       <c r="F6">
+        <v>1E-3</v>
+      </c>
+      <c r="G6">
+        <v>1E-3</v>
+      </c>
+      <c r="H6">
         <v>20</v>
       </c>
-      <c r="G6" s="2">
-        <v>5</v>
-      </c>
-      <c r="H6" s="1">
-        <v>5.9027777777777783E-2</v>
-      </c>
-      <c r="I6" s="1">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="J6">
-        <v>0.23904</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="2">
+        <v>10</v>
+      </c>
+      <c r="J6" s="1">
+        <v>3.4027777777777775E-2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>6.2499999999999995E-3</v>
+      </c>
+      <c r="L6">
+        <v>0.30680000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1138,96 +1176,190 @@
         <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
       </c>
       <c r="F7">
+        <v>1E-3</v>
+      </c>
+      <c r="G7">
+        <v>1E-3</v>
+      </c>
+      <c r="H7">
         <v>20</v>
       </c>
-      <c r="G7" s="2">
-        <v>5</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0.10694444444444444</v>
-      </c>
-      <c r="I7" s="1">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="J7">
-        <v>0.19872000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="2">
+        <v>10</v>
+      </c>
+      <c r="J7" s="1">
+        <v>9.0277777777777776E-2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="L7">
+        <v>0.20108000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+      <c r="E8">
+        <v>9</v>
       </c>
       <c r="F8">
+        <v>1E-3</v>
+      </c>
+      <c r="G8">
+        <v>1E-3</v>
+      </c>
+      <c r="H8">
         <v>20</v>
       </c>
-      <c r="G8" s="2">
-        <v>5</v>
-      </c>
-      <c r="H8" s="1">
-        <v>6.3888888888888884E-2</v>
-      </c>
-      <c r="I8" s="1">
-        <v>2.1527777777777781E-2</v>
-      </c>
-      <c r="J8">
-        <v>0.13252</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="2">
+        <v>10</v>
+      </c>
+      <c r="J8" s="1">
+        <v>7.1527777777777787E-2</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1.4583333333333332E-2</v>
+      </c>
+      <c r="L8">
+        <v>0.15684000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>100</v>
       </c>
       <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>1E-3</v>
+      </c>
+      <c r="G9">
+        <v>1E-3</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
+      <c r="I9" s="2">
+        <v>10</v>
+      </c>
+      <c r="J9" s="1">
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="L9">
+        <v>0.15704000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>1E-3</v>
+      </c>
+      <c r="G10">
+        <v>1E-3</v>
+      </c>
+      <c r="H10">
+        <v>20</v>
+      </c>
+      <c r="I10" s="2">
+        <v>10</v>
+      </c>
+      <c r="J10" s="1">
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="K10" s="1">
+        <v>6.2499999999999995E-3</v>
+      </c>
+      <c r="L10">
+        <v>0.25824000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
         <v>17</v>
       </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9">
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>1E-3</v>
+      </c>
+      <c r="G11">
+        <v>1E-3</v>
+      </c>
+      <c r="H11">
         <v>20</v>
       </c>
-      <c r="G9" s="2">
-        <v>5</v>
-      </c>
-      <c r="H9" s="1">
-        <v>4.7916666666666663E-2</v>
-      </c>
-      <c r="I9" s="1">
-        <v>7.6388888888888886E-3</v>
-      </c>
-      <c r="J9">
-        <v>0.13188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="I11" s="2">
+        <v>10</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2.7083333333333334E-2</v>
+      </c>
+      <c r="K11" s="1">
+        <v>6.2499999999999995E-3</v>
+      </c>
+      <c r="L11">
+        <v>0.11916</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1239,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,8 +1380,7 @@
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="4" max="5" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1257,16 +1388,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
@@ -1274,116 +1405,117 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>0.01</v>
       </c>
       <c r="E2">
-        <v>0.1</v>
+        <v>30</v>
       </c>
       <c r="F2">
-        <v>0.19988</v>
+        <v>0.19819999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>0.01</v>
       </c>
       <c r="E3">
-        <v>0.1</v>
+        <v>30</v>
       </c>
       <c r="F3">
-        <v>0.13303999999999999</v>
+        <v>0.11916</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
       <c r="D4">
-        <v>5</v>
+        <v>0.01</v>
       </c>
       <c r="E4">
-        <v>0.1</v>
+        <v>30</v>
       </c>
       <c r="F4">
-        <v>0.13156000000000001</v>
+        <v>0.12092</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F5">
-        <v>0.13496</v>
+        <v>0.12071999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F6">
-        <v>0.13456000000000001</v>
+        <v>0.12056</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F7">
-        <v>0.13447999999999999</v>
+        <v>0.12092</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dbow frequent word sampling & slightly better results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="30">
   <si>
     <t>method</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t>w2v 1e-2</t>
   </si>
 </sst>
 </file>
@@ -920,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,8 +1374,8 @@
       <c r="D12" t="s">
         <v>17</v>
       </c>
-      <c r="E12">
-        <v>10</v>
+      <c r="E12" t="s">
+        <v>17</v>
       </c>
       <c r="F12">
         <v>1E-3</v>
@@ -1409,8 +1412,8 @@
       <c r="D13" t="s">
         <v>17</v>
       </c>
-      <c r="E13">
-        <v>10</v>
+      <c r="E13" t="s">
+        <v>17</v>
       </c>
       <c r="F13">
         <v>1E-3</v>
@@ -1434,8 +1437,157 @@
         <v>0.13272</v>
       </c>
     </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>1E-3</v>
+      </c>
+      <c r="G14">
+        <v>1E-3</v>
+      </c>
+      <c r="H14">
+        <v>20</v>
+      </c>
+      <c r="I14" s="2">
+        <v>10</v>
+      </c>
+      <c r="J14" s="1">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="K14" s="1">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="L14">
+        <v>0.11935999999999999</v>
+      </c>
+    </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15">
+        <v>1E-3</v>
+      </c>
+      <c r="G15">
+        <v>1E-3</v>
+      </c>
+      <c r="H15">
+        <v>20</v>
+      </c>
+      <c r="I15" s="2">
+        <v>10</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="K15" s="1">
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="L15">
+        <v>0.11744</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16">
+        <v>1E-3</v>
+      </c>
+      <c r="G16">
+        <v>1E-3</v>
+      </c>
+      <c r="H16">
+        <v>20</v>
+      </c>
+      <c r="I16" s="2">
+        <v>10</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1.4583333333333332E-2</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="L16">
+        <v>0.12923999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>100</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17">
+        <v>1E-3</v>
+      </c>
+      <c r="G17">
+        <v>1E-3</v>
+      </c>
+      <c r="H17">
+        <v>20</v>
+      </c>
+      <c r="I17" s="2">
+        <v>10</v>
+      </c>
+      <c r="J17" s="1">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="K17" s="1">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="L17">
+        <v>0.23119999999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>